<commit_message>
Transformations applied and compared
</commit_message>
<xml_diff>
--- a/Tests/xml_values_line_by_line.xlsx
+++ b/Tests/xml_values_line_by_line.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,6 +437,11 @@
           <t>CSV File Fields</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>XML File Fields Transformed</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -452,6 +457,14 @@
       <c r="C2" t="n">
         <v>2002</v>
       </c>
+      <c r="D2" t="n">
+        <v>2002</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -466,7 +479,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Confirmed</t>
+          <t>PROCESSING</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>PROCESSING</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -484,6 +507,14 @@
       <c r="C4" t="n">
         <v>99999</v>
       </c>
+      <c r="D4" t="n">
+        <v>98765</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Mismatch</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -498,7 +529,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bob Johnson</t>
+          <t>Alice Smith</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Alice Smith</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -515,7 +556,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>bob.j@example.com</t>
+          <t>alice.smith@example.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>alice.smith@example.com</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -531,7 +582,15 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-10430</v>
+        <v>15556789</v>
+      </c>
+      <c r="D7" t="n">
+        <v>15556789</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -550,6 +609,16 @@
           <t>10-04-2025</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>15-03-2025</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Mismatch</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -563,7 +632,15 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>299.99</v>
+        <v>500</v>
+      </c>
+      <c r="D9" t="n">
+        <v>500</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -582,6 +659,16 @@
           <t>USD</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -599,6 +686,16 @@
           <t>Overnight</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Mismatch</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -616,6 +713,16 @@
           <t>OVN123987654</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>STD987654321</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Mismatch</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -633,6 +740,16 @@
           <t>789 Pine Street</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>456 Oak Street</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Mismatch</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -647,7 +764,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -664,7 +791,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -680,7 +817,15 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>60601</v>
+        <v>90001</v>
+      </c>
+      <c r="D16" t="n">
+        <v>90001</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -699,6 +844,16 @@
           <t>USA</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -714,6 +869,14 @@
       <c r="C18" t="n">
         <v>1</v>
       </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -727,7 +890,15 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>88888</v>
+        <v>55555</v>
+      </c>
+      <c r="D19" t="n">
+        <v>55555</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -743,7 +914,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Gaming Mouse</t>
+          <t>BlutoothSpeaker</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Bluetooth Speaker</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Mismatch</t>
         </is>
       </c>
     </row>
@@ -760,7 +941,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Accessories</t>
+          <t>Audio</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Audio</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -778,6 +969,16 @@
       <c r="C22" t="n">
         <v>2</v>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Mismatch</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -791,7 +992,15 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>49.99</v>
+        <v>100</v>
+      </c>
+      <c r="D23" t="n">
+        <v>100</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -810,6 +1019,16 @@
           <t>USD</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -825,6 +1044,16 @@
       <c r="C25" t="n">
         <v>5</v>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Mismatch</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -839,6 +1068,16 @@
       </c>
       <c r="C26" t="n">
         <v>5</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Mismatch</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>